<commit_message>
Added basic structure of  Peak Non Peak Feature
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -8,9 +8,10 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="AddProductCategory1" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="AddCustomer" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="AddOrder" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Customer" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="AddOrder" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -31,6 +32,63 @@
   </si>
   <si>
     <t xml:space="preserve">Web Data 67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak_Non_Peak Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEAK_NON_PEAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEEKDAY_BASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECIAL_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOLIDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME_BASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tommy Allen</t>
   </si>
 </sst>
 </file>
@@ -120,19 +178,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -153,52 +211,55 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="21.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="5.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="4.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="4.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="3.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="4.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="3.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.37"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.36"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F4" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -219,34 +280,97 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="4.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="4.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="3.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="4.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="3.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -267,6 +391,74 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="8.82"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
@@ -275,49 +467,46 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="5.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="6.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="11.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="12.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="7.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="16.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="7.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="16.76"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="K1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="S1" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Create Pricing and Category and Product for Peak NonPeak Feature
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -5,13 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Product" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Customer" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="AddOrder" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Order" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -31,27 +31,36 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
+    <t xml:space="preserve">Web Data 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak_Non_Peak Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PEAK_NON_PEAK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEEKDAY_BASED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPECIAL_DAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HOLIDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TIME_BASED</t>
+  </si>
+  <si>
     <t xml:space="preserve">Web Data 67</t>
   </si>
   <si>
-    <t xml:space="preserve">Peak_Non_Peak Price</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PEAK_NON_PEAK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WEEKDAY_BASED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPECIAL_DAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HOLIDAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TIME_BASED</t>
-  </si>
-  <si>
     <t xml:space="preserve">Peak Category</t>
   </si>
   <si>
@@ -59,6 +68,12 @@
   </si>
   <si>
     <t xml:space="preserve">Plan Peak Product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
   </si>
   <si>
     <t xml:space="preserve">Plan Peak Category</t>
@@ -211,22 +226,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="8.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="8.36"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6037037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3925925925926"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -245,20 +262,26 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F3" s="2" t="s">
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="0" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F4" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G4" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -267,7 +290,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -282,27 +305,27 @@
   </sheetPr>
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="15.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="17.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="4.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="4.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="3.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="4.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="3.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="8.82"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8925925925926"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.7777777777778"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.8333333333333"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.01851851851852"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.7037037037037"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="3.82222222222222"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="3.91851851851852"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="4.7037037037037"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="3.91851851851852"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -313,7 +336,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -322,16 +345,20 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
+        <v>14</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>16</v>
+      </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -339,37 +366,37 @@
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="2" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="2" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -378,7 +405,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -393,18 +420,18 @@
   </sheetPr>
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="13.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="8.82"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,29 +442,29 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E4" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -446,7 +473,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -461,30 +488,30 @@
   </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="20.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="6.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="13.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="11.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="12.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="7.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="16.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="8.82"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.7740740740741"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.6814814814815"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="12.4444444444444"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.29259259259259"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.15185185185185"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.5222222222222"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.1481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,7 +522,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
@@ -514,7 +541,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Create Category and Product for Peak NonPeak Feature
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -58,49 +58,52 @@
     <t xml:space="preserve">TIME_BASED</t>
   </si>
   <si>
+    <t xml:space="preserve">Peak Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Web Data 67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Product1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Product1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Product2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Product2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Product3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Product3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Product4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Product4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Product5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Product5</t>
   </si>
   <si>
     <t xml:space="preserve">Tommy Allen</t>
@@ -234,13 +237,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.52592592592593"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6037037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.3925925925926"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.0259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.52592592592593"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.9518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1074074074074"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9555555555556"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81851851851852"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,26 +309,26 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.6"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="19.8925925925926"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="15.7777777777778"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="17.8333333333333"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="4.01851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.7037037037037"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.6555555555556"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.8740740740741"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.5592592592593"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6185185185185"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.62222222222222"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.9"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="3.82222222222222"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="4.7037037037037"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="4.9"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -336,7 +339,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>3</v>
@@ -345,19 +348,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
@@ -366,12 +369,15 @@
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="J2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -426,12 +432,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.7"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -442,10 +448,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -494,24 +500,24 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.7740740740741"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.6814814814815"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="12.4444444444444"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.29259259259259"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.15185185185185"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.5222222222222"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.1481481481481"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.8518518518519"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2481481481481"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.40740740740741"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.2703703703704"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.48888888888889"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.34814814814815"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.0703703703704"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.1111111111111"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.6407407407407"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.64444444444445"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.9333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.40740740740741"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -522,7 +528,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>

</xml_diff>

<commit_message>
Created Peak and non Peak Intervals At company and Product Level
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -46,18 +46,36 @@
     <t xml:space="preserve">WEEKDAY_BASED</t>
   </si>
   <si>
+    <t xml:space="preserve">04/10/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/10/2018</t>
+  </si>
+  <si>
     <t xml:space="preserve">10</t>
   </si>
   <si>
     <t xml:space="preserve">SPECIAL_DAY</t>
   </si>
   <si>
+    <t xml:space="preserve">04/07/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07/15/2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">HOLIDAY</t>
   </si>
   <si>
+    <t xml:space="preserve">09/15/2016</t>
+  </si>
+  <si>
     <t xml:space="preserve">TIME_BASED</t>
   </si>
   <si>
+    <t xml:space="preserve">03/10/2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peak Category</t>
   </si>
   <si>
@@ -67,24 +85,36 @@
     <t xml:space="preserve">Plan Peak Product1</t>
   </si>
   <si>
+    <t xml:space="preserve">Items</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TUESDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product2</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plan</t>
   </si>
   <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Product2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Product2</t>
-  </si>
-  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
+    <t xml:space="preserve">FRIDAY</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peak Product3</t>
   </si>
   <si>
@@ -103,19 +133,48 @@
     <t xml:space="preserve">Plan Peak Product5</t>
   </si>
   <si>
+    <t xml:space="preserve">Peak Product6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product6</t>
+  </si>
+  <si>
     <t xml:space="preserve">Web Data 67</t>
   </si>
   <si>
     <t xml:space="preserve">Tommy Allen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nancy Winters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyler Kim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo Holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betsy Klompus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin Bernstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warren Drummond</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -191,7 +250,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -204,11 +263,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -229,21 +296,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.9518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1074074074074"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.9555555555556"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.4"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81851851851852"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.82"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -268,23 +337,41 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F2" s="0" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -293,7 +380,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -306,32 +393,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.2888888888889"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.6555555555556"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="20.8740740740741"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.5592592592593"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.6185185185185"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.62222222222222"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.9"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="3.82222222222222"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="4.9"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="3.91851851851852"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="9.40740740740741"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="9.41"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -345,64 +432,96 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="N2" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E3" s="0"/>
       <c r="G3" s="2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="2" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="2" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>25</v>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -411,7 +530,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -424,20 +543,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.7"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="1" width="9.40740740740741"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -448,10 +567,10 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -459,18 +578,47 @@
       <c r="F1" s="2"/>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D2" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="E2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D3" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -479,7 +627,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -494,52 +642,52 @@
   </sheetPr>
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.8518518518519"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.2481481481481"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.40740740740741"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.2703703703704"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="5.48888888888889"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.34814814814815"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.0703703703704"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.1111111111111"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.6407407407407"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.64444444444445"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="17.9333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.40740740740741"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="7.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="9.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="S1" s="4"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -547,7 +695,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added the Customer Level Peak Non-Peak Interval Scenario
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -139,9 +139,6 @@
     <t xml:space="preserve">Plan Peak Product6</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 67</t>
-  </si>
-  <si>
     <t xml:space="preserve">Tommy Allen</t>
   </si>
   <si>
@@ -164,17 +161,37 @@
   </si>
   <si>
     <t xml:space="preserve">Warren Drummond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$30.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04/09/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$50.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$40.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$15.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="167" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -275,7 +292,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -298,8 +315,8 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K10" activeCellId="0" sqref="K10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,7 +413,7 @@
   <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -543,10 +560,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -556,10 +573,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.41"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -567,58 +585,78 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -640,10 +678,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:S1"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -653,10 +691,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="9.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.07"/>
@@ -676,18 +715,132 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="E1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
       <c r="S1" s="6"/>
+    </row>
+    <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D5" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I6" s="2"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I8" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added Validation at Product Level Peak
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -97,6 +97,21 @@
     <t xml:space="preserve">TUESDAY</t>
   </si>
   <si>
+    <t xml:space="preserve">Apr 10, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Apr 10, 2018</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
+  </si>
+  <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:00:00</t>
+  </si>
+  <si>
     <t xml:space="preserve">Plan Peak Category</t>
   </si>
   <si>
@@ -113,6 +128,18 @@
   </si>
   <si>
     <t xml:space="preserve">FRIDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar 10, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jul 15, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18:00:00</t>
   </si>
   <si>
     <t xml:space="preserve">Peak Product3</t>
@@ -315,21 +342,21 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="8.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="29.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="15.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.82"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.01481481481481"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4407407407407"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2481481481481"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.0851851851852"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2074074074074"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2666666666667"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.01481481481481"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -397,7 +424,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -410,29 +437,31 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="18.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="4.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="16.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="15" style="1" width="9.41"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7185185185185"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.2444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.362962962963"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.9518518518519"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.0111111111111"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.81851851851852"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.9962962962963"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.3444444444444"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.0518518518519"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1518518518519"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.5444444444444"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.7074074074074"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.2148148148148"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -478,25 +507,43 @@
       <c r="N1" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="O1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>16</v>
@@ -505,40 +552,76 @@
         <v>12</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>34</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="0"/>
       <c r="G3" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>31</v>
+        <v>40</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +630,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -562,19 +645,19 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.41"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9925925925926"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="14.8962962962963"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -588,7 +671,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>6</v>
@@ -605,7 +688,7 @@
     </row>
     <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>10</v>
@@ -619,7 +702,7 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>13</v>
@@ -630,7 +713,7 @@
     </row>
     <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>15</v>
@@ -641,22 +724,22 @@
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -665,7 +748,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -680,31 +763,31 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.76"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="12.84"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="7.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="17.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="9.41"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.6037037037037"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.3444444444444"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6407407407407"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.2074074074074"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.562962962963"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.9"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1296296296296"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6777777777778"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.44814814814815"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.462962962963"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.4037037037037"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.837037037037"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.4259259259259"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.74074074074074"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="18.3259259259259"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.6037037037037"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -718,7 +801,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>18</v>
@@ -730,13 +813,13 @@
         <v>7</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -745,22 +828,22 @@
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>17</v>
@@ -768,77 +851,77 @@
     </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>31</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="I5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D6" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="I6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="I7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="I8" s="2"/>
     </row>
@@ -848,7 +931,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Product Level Scenario and Validation for products Peak
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="63">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 13</t>
+    <t xml:space="preserve">Web Data 21</t>
   </si>
   <si>
     <t xml:space="preserve">Peak_Non_Peak Price</t>
@@ -103,39 +103,39 @@
     <t xml:space="preserve">Apr 10, 2018</t>
   </si>
   <si>
+    <t xml:space="preserve">false</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peak Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Peak Product2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRIDAY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mar 10, 2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jul 15, 2017</t>
+  </si>
+  <si>
     <t xml:space="preserve">true</t>
   </si>
   <si>
-    <t xml:space="preserve">false</t>
-  </si>
-  <si>
-    <t xml:space="preserve">00:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Peak Product2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Peak Product2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FRIDAY</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mar 10, 2017</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jul 15, 2017</t>
-  </si>
-  <si>
     <t xml:space="preserve">09:00:00</t>
   </si>
   <si>
@@ -193,12 +193,18 @@
     <t xml:space="preserve">US$30.00</t>
   </si>
   <si>
+    <t xml:space="preserve">US$20.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">04/09/2017</t>
   </si>
   <si>
     <t xml:space="preserve">US$50.00</t>
   </si>
   <si>
+    <t xml:space="preserve">US$15.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">4</t>
   </si>
   <si>
@@ -206,9 +212,6 @@
   </si>
   <si>
     <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US$15.00</t>
   </si>
 </sst>
 </file>
@@ -342,21 +345,21 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.01481481481481"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4407407407407"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2481481481481"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.0851851851852"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.2074074074074"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="16.2666666666667"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.01481481481481"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="9.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="30.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="9.01"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -424,7 +427,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -437,31 +440,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6777777777778"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.7185185185185"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.2444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="21.362962962963"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="16.9518518518519"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.0111111111111"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.81851851851852"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="4.9962962962963"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="17.3444444444444"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.0518518518519"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.1518518518519"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="12.5444444444444"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.7074074074074"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.2148148148148"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="9.6037037037037"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="21.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="19.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="8.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="17.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="17.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="12.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="17" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="8.36"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -520,10 +524,7 @@
         <v>27</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -531,19 +532,19 @@
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>16</v>
@@ -552,28 +553,25 @@
         <v>12</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>26</v>
-      </c>
       <c r="R2" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T2" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="0"/>
       <c r="G3" s="2" t="s">
         <v>39</v>
@@ -582,22 +580,19 @@
         <v>40</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>27</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -607,6 +602,11 @@
       <c r="H4" s="2" t="s">
         <v>42</v>
       </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="2" t="s">
@@ -630,7 +630,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -645,19 +645,19 @@
   </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="14.9925925925926"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="14.8962962962963"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="1" width="9.6037037037037"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -748,7 +748,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
@@ -763,31 +763,31 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.6037037037037"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.3444444444444"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.6407407407407"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="19.2074074074074"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.562962962963"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="4.9"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.1296296296296"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6777777777778"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="7.44814814814815"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.462962962963"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="14.4037037037037"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.837037037037"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.4259259259259"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="7.74074074074074"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="18.3259259259259"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="1" width="9.6037037037037"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.84"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="7.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="9.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -813,13 +813,16 @@
         <v>7</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="N1" s="6"/>
       <c r="O1" s="6"/>
@@ -831,22 +834,25 @@
         <v>48</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="G2" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>17</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -863,10 +869,10 @@
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -880,13 +886,13 @@
         <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -931,7 +937,7 @@
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Added Verify and All the Scenario's of the Peak Non Peak Feature
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="70">
   <si>
     <t xml:space="preserve">admin</t>
   </si>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">Web Data 21</t>
+    <t xml:space="preserve">SK Telecom</t>
   </si>
   <si>
     <t xml:space="preserve">Peak_Non_Peak Price</t>
@@ -196,6 +196,12 @@
     <t xml:space="preserve">US$20.00</t>
   </si>
   <si>
+    <t xml:space="preserve">US$150.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3</t>
+  </si>
+  <si>
     <t xml:space="preserve">04/09/2017</t>
   </si>
   <si>
@@ -211,7 +217,22 @@
     <t xml:space="preserve">US$40.00</t>
   </si>
   <si>
+    <t xml:space="preserve">9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$90.00</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$75.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$45.00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US$60.00</t>
   </si>
 </sst>
 </file>
@@ -223,7 +244,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -253,6 +274,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -297,7 +324,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +346,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,7 +377,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -646,7 +677,7 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E22" activeCellId="0" sqref="E22"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -764,25 +795,25 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G23" activeCellId="0" sqref="G23"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="7.74"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="17.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="19.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="13.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="20.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="16.46"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.4"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="18.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="9.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="9.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="2.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="13.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="7.74"/>
@@ -790,14 +821,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="19" style="1" width="9.6"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -812,7 +843,7 @@
       <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>32</v>
       </c>
       <c r="I1" s="2" t="s">
@@ -824,10 +855,18 @@
       <c r="K1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="N1" s="6"/>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="S1" s="6"/>
+      <c r="L1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="S1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="2" t="s">
@@ -840,19 +879,28 @@
         <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>17</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -869,10 +917,19 @@
         <v>14</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -886,13 +943,19 @@
         <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -905,7 +968,13 @@
       <c r="F5" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="I5" s="2"/>
+      <c r="M5" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D6" s="2" t="s">
@@ -918,12 +987,18 @@
         <v>46</v>
       </c>
       <c r="I6" s="2"/>
+      <c r="M6" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="2" t="s">
         <v>53</v>
       </c>
       <c r="I7" s="2"/>
+      <c r="M7" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">

</xml_diff>

<commit_message>
Added Filter for Customer in the Peak Non-Peak Feature
</commit_message>
<xml_diff>
--- a/Peak_Non_Peak_Test_Data.xlsx
+++ b/Peak_Non_Peak_Test_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Pricing" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Customer" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Customer" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Product" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Order" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">WebData@123</t>
   </si>
   <si>
-    <t xml:space="preserve">SK Telecom</t>
+    <t xml:space="preserve">Web Data 6</t>
   </si>
   <si>
     <t xml:space="preserve">Peak_Non_Peak Price</t>
@@ -76,6 +76,33 @@
     <t xml:space="preserve">03/10/2017</t>
   </si>
   <si>
+    <t xml:space="preserve">Tommy Allen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Dollar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">James Wilson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nancy Winters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tyler Kim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leo Holder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betsy Klompus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Martin Bernstein</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Warren Drummond</t>
+  </si>
+  <si>
     <t xml:space="preserve">Peak Category</t>
   </si>
   <si>
@@ -91,9 +118,6 @@
     <t xml:space="preserve">5</t>
   </si>
   <si>
-    <t xml:space="preserve">United States Dollar</t>
-  </si>
-  <si>
     <t xml:space="preserve">TUESDAY</t>
   </si>
   <si>
@@ -164,30 +188,6 @@
   </si>
   <si>
     <t xml:space="preserve">Plan Peak Product6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tommy Allen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">James Wilson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nancy Winters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tyler Kim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leo Holder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Betsy Klompus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martin Bernstein</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Warren Drummond</t>
   </si>
   <si>
     <t xml:space="preserve">US$30.00</t>
@@ -244,7 +244,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -274,12 +274,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -324,7 +318,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -346,10 +340,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -376,8 +366,8 @@
   </sheetPr>
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -471,10 +461,128 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="22.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.6"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -516,22 +624,22 @@
         <v>6</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>7</v>
@@ -540,22 +648,22 @@
         <v>8</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="Q1" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="R1" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -563,19 +671,19 @@
         <v>15</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>16</v>
@@ -584,54 +692,54 @@
         <v>12</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E3" s="0"/>
       <c r="G3" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="R3" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G4" s="2" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="O4" s="2"/>
       <c r="P4" s="2"/>
@@ -641,135 +749,17 @@
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G5" s="2" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G6" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="WebData@123"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H8"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.6"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="22.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="1" width="9.6"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D2" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D3" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="D4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="2" t="s">
         <v>54</v>
       </c>
     </row>
@@ -794,7 +784,7 @@
   </sheetPr>
   <dimension ref="A1:S8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -828,29 +818,29 @@
       <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>32</v>
+      <c r="H1" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>55</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>56</v>
@@ -861,40 +851,40 @@
       <c r="M1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="7"/>
-      <c r="S1" s="7"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="S1" s="6"/>
     </row>
     <row r="2" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>59</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>60</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>61</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>56</v>
@@ -905,13 +895,13 @@
     </row>
     <row r="3" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D3" s="2" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>14</v>
@@ -929,18 +919,18 @@
         <v>65</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>42</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>59</v>
@@ -952,7 +942,7 @@
         <v>61</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>67</v>
@@ -960,13 +950,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>43</v>
-      </c>
       <c r="F5" s="2" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>11</v>
@@ -978,13 +968,13 @@
     </row>
     <row r="6" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="D6" s="2" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="I6" s="2"/>
       <c r="M6" s="2" t="s">
@@ -993,7 +983,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D7" s="2" t="s">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="I7" s="2"/>
       <c r="M7" s="2" t="s">
@@ -1002,7 +992,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D8" s="2" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="I8" s="2"/>
     </row>

</xml_diff>